<commit_message>
added data for better display of expiration filter
</commit_message>
<xml_diff>
--- a/addons/pharma-pos/demo_excel/deliveries/pharma_pos.batch.xlsx
+++ b/addons/pharma-pos/demo_excel/deliveries/pharma_pos.batch.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Product</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -399,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -465,7 +468,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>44958</v>
+        <v>44608</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -486,6 +489,26 @@
       </c>
       <c r="F4" s="3">
         <v>44958</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>44608</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated to become importable due to the changes in Batch record string representation
</commit_message>
<xml_diff>
--- a/addons/pharma-pos/demo_excel/deliveries/pharma_pos.batch.xlsx
+++ b/addons/pharma-pos/demo_excel/deliveries/pharma_pos.batch.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Product</t>
   </si>
@@ -31,6 +31,9 @@
     <t>Packs Left</t>
   </si>
   <si>
+    <t>Packs Unboxed</t>
+  </si>
+  <si>
     <t>Expiration Date</t>
   </si>
   <si>
@@ -59,6 +62,27 @@
   </si>
   <si>
     <t>77</t>
+  </si>
+  <si>
+    <t>(Aciclovir) 200 mg Tablet 5x: ₱5.0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Mucosolve (Ambroxol) 15 mg/60 ml Syrup 1x: ₱9.0</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>(Allopurinol) 100 mg Tablet 10x: ₱2.0</t>
+  </si>
+  <si>
+    <t>456</t>
+  </si>
+  <si>
+    <t>5678</t>
   </si>
 </sst>
 </file>
@@ -408,16 +432,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="6" width="30.7109375" customWidth="1"/>
+    <col min="1" max="7" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,13 +460,16 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2">
         <v>10</v>
@@ -453,16 +480,19 @@
       <c r="E2" s="2">
         <v>10</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
         <v>44253</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2">
         <v>7</v>
@@ -473,16 +503,19 @@
       <c r="E3" s="2">
         <v>7</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
         <v>44244</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2">
         <v>8</v>
@@ -493,16 +526,19 @@
       <c r="E4" s="2">
         <v>8</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
         <v>44259</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2">
         <v>6</v>
@@ -513,16 +549,19 @@
       <c r="E5" s="2">
         <v>6</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
         <v>44249</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2">
         <v>7</v>
@@ -533,8 +572,126 @@
       <c r="E6" s="2">
         <v>7</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
         <v>44235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>44239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>44246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>44242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>9</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>44244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>6</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>44251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>